<commit_message>
Cập nhật Giao diện và sửa lỗi
</commit_message>
<xml_diff>
--- a/BiTech.Library/BiTech.Library/Tempalates/ExportTTSach.xlsx
+++ b/BiTech.Library/BiTech.Library/Tempalates/ExportTTSach.xlsx
@@ -2,47 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>maks</t>
-  </si>
-  <si>
-    <t>ten sach</t>
-  </si>
-  <si>
-    <t>sdfs</t>
-  </si>
-  <si>
-    <t>dsf</t>
-  </si>
-  <si>
-    <t>sl tong</t>
-  </si>
-  <si>
-    <t>sl sach ko cho muon</t>
-  </si>
-  <si>
-    <t>sl cho muon</t>
-  </si>
-  <si>
-    <t>STATUS TRUE</t>
-  </si>
-  <si>
-    <t>STATUS FALSE</t>
+    <t>Tháng</t>
   </si>
   <si>
     <t>Số lượng sách được mượn</t>
@@ -51,14 +27,14 @@
     <t>Số lượng người mượn sách</t>
   </si>
   <si>
-    <t>Tháng</t>
+    <t>Bảng Thống Kê Số  Sách  số người mượn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +44,21 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -110,10 +101,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,279 +407,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A2:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="D1" t="s">
-        <v>7</v>
+    <row r="2" spans="1:5" ht="18.75">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>1000</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>34</v>
-      </c>
-      <c r="D3">
-        <v>34</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>1000</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>434</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5">
-        <v>1000</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>43</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6">
-        <v>1000</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>43</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7">
-        <v>1000</v>
-      </c>
-      <c r="D7">
-        <v>34</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8">
-        <v>1000</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>43</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9">
-        <v>1000</v>
-      </c>
-      <c r="D9">
-        <v>34</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10">
-        <v>1000</v>
-      </c>
-      <c r="D10">
-        <v>34</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11">
-        <v>1000</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D14"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="6.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" ht="15.75">
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4">
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="1">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="1">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="1">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="1">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="1">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="1">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="1">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="1">
-        <v>10</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="1">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="1">
-        <v>12</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>